<commit_message>
added puff-time showing arrows on graph
</commit_message>
<xml_diff>
--- a/Protocol/IschemiaProtocol.xlsx
+++ b/Protocol/IschemiaProtocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -96,15 +96,6 @@
   </si>
   <si>
     <t>\\IFMB-02-024B-10\Ischemia2\IOS\2019-05-30\2019-05-30_16-13-12.ios</t>
-  </si>
-  <si>
-    <t>\\IFMB-02-024B-07\Ischemia\151117_P17\151117_P17_slc2_2000.abf</t>
-  </si>
-  <si>
-    <t>\\ED03\MMarat\IOS_Ischemia\2017-11-15\2017-11-15_13-40-27.ios</t>
-  </si>
-  <si>
-    <t>151117_P17_slc2</t>
   </si>
   <si>
     <t>\\IFMB-02-024B-10\Ischemia2\300519_P17_SD\300519_P17_slc4_4000.abf</t>
@@ -201,7 +192,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,35 +208,16 @@
       <name val="Arial Cyr"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Cyr"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -253,33 +225,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -296,24 +247,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Акцент5" xfId="2" builtinId="45"/>
+  <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -410,8 +345,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:O15" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:O14" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O14"/>
   <tableColumns count="15">
     <tableColumn id="12" name="ID" dataDxfId="14"/>
     <tableColumn id="1" name="name" dataDxfId="13"/>
@@ -696,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,28 +757,27 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>280</v>
-      </c>
-      <c r="B5" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>17</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3">
         <v>17</v>
@@ -852,174 +786,155 @@
         <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3">
         <v>17</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3">
         <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3">
         <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3">
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" s="3">
         <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="4" t="s">
         <v>45</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" s="3">
         <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C14" s="3">
         <v>15</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>503</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="3">
-        <v>15</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="F5" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E11" r:id="rId4"/>
-    <hyperlink ref="F12" r:id="rId5"/>
-    <hyperlink ref="E15" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="F11" r:id="rId3"/>
+    <hyperlink ref="E14" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
difference beween time of creation of OIS and LFP files detected by find_lost_time function changed names of data subfolders ios_trace to OIS_trace made one single method for reading OIS data with readOOS and readIOS.
</commit_message>
<xml_diff>
--- a/Protocol/IschemiaProtocol.xlsx
+++ b/Protocol/IschemiaProtocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>name</t>
   </si>
@@ -222,6 +222,153 @@
   </si>
   <si>
     <t>100619_P29_slc3_3002</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\110619_P26\1110619_P26_slc1_1000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\IOS\2019-06-11\2019-06-11_12-51-28.ios</t>
+  </si>
+  <si>
+    <t>1110619_P26_slc1</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\110619_P26_SD\100619_P29_slc2_2001.abf</t>
+  </si>
+  <si>
+    <t>110619_P26_slc2_2001</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\IOS\2019-06-11\2019-06-11_14-21-31.ios</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-11\2019-06-11_16-9-55.oos</t>
+  </si>
+  <si>
+    <t>110619_P26_slc4</t>
+  </si>
+  <si>
+    <t>\\ifmb-02-024b-10\Ischemia2\110619_P26_SD\110619_P26_slc4_4000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_10-40-37.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1000.abf</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1000</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1001.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1002.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_11-33-7.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1003.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1004.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_11-47-26.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_11-53-26.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1005.abf</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1001</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1002</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1003</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1004</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1005</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1006.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_12-16-9.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc1_1007.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_12-44-36.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc2_2000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_13-53-29.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_14-25-38.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc3_cell 1_3000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_15-34-43.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc3_cell 2_3002.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_15-48-15.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc4_cell 1_4000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_16-29-37.oos</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1006</t>
+  </si>
+  <si>
+    <t>130619_P14_slc1_1007</t>
+  </si>
+  <si>
+    <t>130619_P14_slc2_2000</t>
+  </si>
+  <si>
+    <t>130619_P14_slc3_cell 1_3000</t>
+  </si>
+  <si>
+    <t>130619_P14_slc3_cell 2_3002</t>
+  </si>
+  <si>
+    <t>130619_P14_slc4_cell 1_4000</t>
+  </si>
+  <si>
+    <t>130619_P14_slc2_cell 2_0000</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc2_cell 2_0000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\130619_P14_SD\130619_P14_slc5_cell 1_5000.abf</t>
+  </si>
+  <si>
+    <t>130619_P14_slc5_cell 1_5000</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-06-13\2019-06-13_17-11-34.oos</t>
   </si>
 </sst>
 </file>
@@ -381,8 +528,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:O18" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:O35" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O35"/>
   <tableColumns count="15">
     <tableColumn id="12" name="ID" dataDxfId="14"/>
     <tableColumn id="1" name="name" dataDxfId="13"/>
@@ -667,16 +814,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="5.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="26.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
@@ -1029,6 +1176,291 @@
         <v>64</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>508</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="3">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>509</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3">
+        <v>26</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>510</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="3">
+        <v>26</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>511</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="3">
+        <v>14</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>512</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="3">
+        <v>14</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>513</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="3">
+        <v>14</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>514</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3">
+        <v>14</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>515</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="3">
+        <v>14</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>516</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="3">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>517</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="3">
+        <v>14</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>518</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="3">
+        <v>14</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>519</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="3">
+        <v>14</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>520</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="3">
+        <v>14</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>521</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="3">
+        <v>14</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>522</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="3">
+        <v>14</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>523</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="3">
+        <v>14</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>524</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="3">
+        <v>14</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1"/>
@@ -1036,10 +1468,18 @@
     <hyperlink ref="E14" r:id="rId3"/>
     <hyperlink ref="E16" r:id="rId4"/>
     <hyperlink ref="E17" r:id="rId5"/>
+    <hyperlink ref="E19" r:id="rId6"/>
+    <hyperlink ref="E20" r:id="rId7"/>
+    <hyperlink ref="F20" r:id="rId8"/>
+    <hyperlink ref="E21" r:id="rId9"/>
+    <hyperlink ref="E33" r:id="rId10"/>
+    <hyperlink ref="E34" r:id="rId11"/>
+    <hyperlink ref="E31" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
clean parts of LFP signal and OIS at epilepsy has been analysed average power of OIS and LFP compared
</commit_message>
<xml_diff>
--- a/Protocol/IschemiaProtocol.xlsx
+++ b/Protocol/IschemiaProtocol.xlsx
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1502,11 +1502,12 @@
     <hyperlink ref="E34" r:id="rId11"/>
     <hyperlink ref="E31" r:id="rId12"/>
     <hyperlink ref="E36" r:id="rId13"/>
+    <hyperlink ref="E13" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>